<commit_message>
Added information about working hours in 2023.
</commit_message>
<xml_diff>
--- a/Parameters/WHours.xlsx
+++ b/Parameters/WHours.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A55BDD-3E7C-4863-BDE0-758197371160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995EE396-DED7-45CB-8652-B33EF032CE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>07. Июл 2020</t>
   </si>
@@ -134,13 +134,49 @@
   </si>
   <si>
     <t>FirstDate</t>
+  </si>
+  <si>
+    <t>01. Янв 2023</t>
+  </si>
+  <si>
+    <t>02. Фев 2023</t>
+  </si>
+  <si>
+    <t>03. Мар 2023</t>
+  </si>
+  <si>
+    <t>04. Апр 2023</t>
+  </si>
+  <si>
+    <t>05. Май 2023</t>
+  </si>
+  <si>
+    <t>06. Июн 2023</t>
+  </si>
+  <si>
+    <t>07. Июл 2023</t>
+  </si>
+  <si>
+    <t>08. Авг 2023</t>
+  </si>
+  <si>
+    <t>09. Сен 2023</t>
+  </si>
+  <si>
+    <t>10. Окт 2023</t>
+  </si>
+  <si>
+    <t>11. Ноя 2023</t>
+  </si>
+  <si>
+    <t>12. Дек 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +187,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,8 +236,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -478,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -486,25 +528,25 @@
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1050,69 +1092,223 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="A32" s="1">
+        <v>44927</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2" t="str">
+        <f t="shared" ref="C32:C43" si="1">TEXT(A32,"МММ")</f>
+        <v>янв</v>
+      </c>
+      <c r="D32" s="3">
+        <v>136</v>
+      </c>
+      <c r="E32" s="3">
+        <v>122.4</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="A33" s="1">
+        <v>44958</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>фев</v>
+      </c>
+      <c r="D33" s="3">
+        <v>143</v>
+      </c>
+      <c r="E33" s="3">
+        <v>128.6</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="A34" s="1">
+        <v>44986</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>мар</v>
+      </c>
+      <c r="D34" s="3">
+        <v>175</v>
+      </c>
+      <c r="E34" s="3">
+        <v>157.4</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="A35" s="1">
+        <v>45017</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>апр</v>
+      </c>
+      <c r="D35" s="3">
+        <v>160</v>
+      </c>
+      <c r="E35" s="3">
+        <v>144</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="A36" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>май</v>
+      </c>
+      <c r="D36" s="3">
+        <v>160</v>
+      </c>
+      <c r="E36" s="3">
+        <v>144</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="A37" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>июн</v>
+      </c>
+      <c r="D37" s="3">
+        <v>168</v>
+      </c>
+      <c r="E37" s="3">
+        <v>151.19999999999999</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="A38" s="1">
+        <v>45108</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>июл</v>
+      </c>
+      <c r="D38" s="3">
+        <v>168</v>
+      </c>
+      <c r="E38" s="3">
+        <v>151.19999999999999</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="A39" s="1">
+        <v>45139</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>авг</v>
+      </c>
+      <c r="D39" s="3">
+        <v>184</v>
+      </c>
+      <c r="E39" s="3">
+        <v>165.6</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="A40" s="1">
+        <v>45170</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>сен</v>
+      </c>
+      <c r="D40" s="3">
+        <v>168</v>
+      </c>
+      <c r="E40" s="3">
+        <v>151.19999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>45200</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>окт</v>
+      </c>
+      <c r="D41" s="3">
+        <v>176</v>
+      </c>
+      <c r="E41" s="3">
+        <v>158.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>45231</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>ноя</v>
+      </c>
+      <c r="D42" s="3">
+        <v>167</v>
+      </c>
+      <c r="E42" s="3">
+        <v>150.19999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>45261</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>дек</v>
+      </c>
+      <c r="D43" s="3">
+        <v>168</v>
+      </c>
+      <c r="E43" s="3">
+        <v>151.19999999999999</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>